<commit_message>
tempory save for 记忆
</commit_message>
<xml_diff>
--- a/summary/accuracy_summary.xlsx
+++ b/summary/accuracy_summary.xlsx
@@ -130,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -141,6 +141,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -425,7 +428,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -439,32 +442,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5" t="s">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
@@ -479,12 +482,18 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
       </c>
+      <c r="C4" s="1">
+        <v>0.75596814999999995</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.75596814999999995</v>
+      </c>
       <c r="E4" s="3">
         <v>0.77200000000000002</v>
       </c>
@@ -493,10 +502,16 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="2">
         <v>2</v>
       </c>
+      <c r="C5" s="1">
+        <v>0.76373625000000001</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.75274724000000004</v>
+      </c>
       <c r="E5" s="3">
         <v>0.75</v>
       </c>
@@ -505,10 +520,16 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
+      <c r="A6" s="6"/>
       <c r="B6" s="2">
         <v>3</v>
       </c>
+      <c r="C6" s="1">
+        <v>0.76216214999999998</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.77297300000000002</v>
+      </c>
       <c r="E6" s="3">
         <v>0.74199999999999999</v>
       </c>
@@ -517,10 +538,16 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
+      <c r="A7" s="6"/>
       <c r="B7" s="2">
         <v>4</v>
       </c>
+      <c r="C7" s="1">
+        <v>0.73949580000000004</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.75350139999999999</v>
+      </c>
       <c r="E7" s="3">
         <v>0.747</v>
       </c>
@@ -529,10 +556,16 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="2">
         <v>5</v>
       </c>
+      <c r="C8" s="1">
+        <v>0.77235770000000004</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.77235770000000004</v>
+      </c>
       <c r="E8" s="3">
         <v>0.745</v>
       </c>
@@ -541,10 +574,16 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
+      <c r="A9" s="6"/>
       <c r="B9" s="2">
         <v>6</v>
       </c>
+      <c r="C9" s="1">
+        <v>0.75741239999999999</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.74123989999999995</v>
+      </c>
       <c r="E9" s="3">
         <v>0.79900000000000004</v>
       </c>
@@ -553,10 +592,16 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
+      <c r="A10" s="6"/>
       <c r="B10" s="2">
         <v>7</v>
       </c>
+      <c r="C10" s="1">
+        <v>0.76151764</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.7506775</v>
+      </c>
       <c r="E10" s="3">
         <v>0.75800000000000001</v>
       </c>
@@ -565,10 +610,16 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
+      <c r="A11" s="6"/>
       <c r="B11" s="2">
         <v>8</v>
       </c>
+      <c r="C11" s="1">
+        <v>0.75136614000000002</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.70218579999999997</v>
+      </c>
       <c r="E11" s="3">
         <v>0.78800000000000003</v>
       </c>
@@ -577,10 +628,16 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
+      <c r="A12" s="6"/>
       <c r="B12" s="2">
         <v>9</v>
       </c>
+      <c r="C12" s="1">
+        <v>0.78571427000000005</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.77197800000000005</v>
+      </c>
       <c r="E12" s="3">
         <v>0.77200000000000002</v>
       </c>
@@ -589,10 +646,16 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
+      <c r="A13" s="6"/>
       <c r="B13" s="2">
         <v>10</v>
       </c>
+      <c r="C13" s="1">
+        <v>0.75842695999999998</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.77247189999999999</v>
+      </c>
       <c r="E13" s="3">
         <v>0.77200000000000002</v>
       </c>
@@ -601,9 +664,17 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
+      <c r="A14" s="6"/>
       <c r="B14" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="C14" s="5">
+        <f>AVERAGE(C4:C13)</f>
+        <v>0.76081574600000013</v>
+      </c>
+      <c r="D14" s="5">
+        <f>AVERAGE(D4:D13)</f>
+        <v>0.75461005899999989</v>
       </c>
       <c r="E14" s="2">
         <f>AVERAGE(E4:E13)</f>
@@ -615,7 +686,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B15" s="2">
@@ -631,7 +702,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
+      <c r="A16" s="6"/>
       <c r="B16" s="2">
         <v>2</v>
       </c>
@@ -645,7 +716,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
+      <c r="A17" s="6"/>
       <c r="B17" s="2">
         <v>3</v>
       </c>
@@ -659,7 +730,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
+      <c r="A18" s="6"/>
       <c r="B18" s="2">
         <v>4</v>
       </c>
@@ -673,7 +744,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
+      <c r="A19" s="6"/>
       <c r="B19" s="2">
         <v>5</v>
       </c>
@@ -687,7 +758,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
+      <c r="A20" s="6"/>
       <c r="B20" s="2">
         <v>6</v>
       </c>
@@ -701,7 +772,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
+      <c r="A21" s="6"/>
       <c r="B21" s="2">
         <v>7</v>
       </c>
@@ -715,7 +786,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
+      <c r="A22" s="6"/>
       <c r="B22" s="2">
         <v>8</v>
       </c>
@@ -729,7 +800,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="5"/>
+      <c r="A23" s="6"/>
       <c r="B23" s="2">
         <v>9</v>
       </c>
@@ -743,7 +814,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
+      <c r="A24" s="6"/>
       <c r="B24" s="2">
         <v>10</v>
       </c>
@@ -757,7 +828,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
+      <c r="A25" s="6"/>
       <c r="B25" s="2" t="s">
         <v>6</v>
       </c>

</xml_diff>